<commit_message>
Comit: Ya guarda Unidad.java, falta ajustar los contraladores y establecer el mismo modelo que Unidad.java
</commit_message>
<xml_diff>
--- a/src/main/resources/db/1.xlsx
+++ b/src/main/resources/db/1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dev\GIT\sisfubackend\src\main\resources\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D68AD060-6B0F-488D-85A5-A08771D897B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1043787C-99C4-49D1-B249-97CE551A4837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="769" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1553,6 +1553,51 @@
     <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1568,51 +1613,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1622,6 +1622,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1639,24 +1657,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3793,24 +3793,24 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A27:A32"/>
+    <mergeCell ref="B27:B32"/>
+    <mergeCell ref="C27:C32"/>
+    <mergeCell ref="A21:A26"/>
+    <mergeCell ref="B21:B26"/>
+    <mergeCell ref="C21:C26"/>
+    <mergeCell ref="C3:C14"/>
+    <mergeCell ref="A3:A14"/>
+    <mergeCell ref="B3:B14"/>
+    <mergeCell ref="A15:A20"/>
+    <mergeCell ref="B15:B20"/>
+    <mergeCell ref="C15:C20"/>
     <mergeCell ref="A33:A38"/>
     <mergeCell ref="B33:B38"/>
     <mergeCell ref="C33:C38"/>
     <mergeCell ref="A39:A44"/>
     <mergeCell ref="B39:B44"/>
     <mergeCell ref="C39:C44"/>
-    <mergeCell ref="C3:C14"/>
-    <mergeCell ref="A3:A14"/>
-    <mergeCell ref="B3:B14"/>
-    <mergeCell ref="A15:A20"/>
-    <mergeCell ref="B15:B20"/>
-    <mergeCell ref="C15:C20"/>
-    <mergeCell ref="A27:A32"/>
-    <mergeCell ref="B27:B32"/>
-    <mergeCell ref="C27:C32"/>
-    <mergeCell ref="A21:A26"/>
-    <mergeCell ref="B21:B26"/>
-    <mergeCell ref="C21:C26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3824,7 +3824,7 @@
     <sheetView showGridLines="0" tabSelected="1" zoomScale="95" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="R16" sqref="R16"/>
+      <selection pane="topRight" activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -5769,72 +5769,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="37.5" customHeight="1">
-      <c r="B1" s="86" t="s">
+      <c r="B1" s="101" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
-      <c r="F1" s="86"/>
-      <c r="G1" s="86"/>
-      <c r="H1" s="86"/>
-      <c r="I1" s="86"/>
-      <c r="J1" s="86"/>
-      <c r="K1" s="86"/>
-      <c r="L1" s="86"/>
+      <c r="C1" s="101"/>
+      <c r="D1" s="101"/>
+      <c r="E1" s="101"/>
+      <c r="F1" s="101"/>
+      <c r="G1" s="101"/>
+      <c r="H1" s="101"/>
+      <c r="I1" s="101"/>
+      <c r="J1" s="101"/>
+      <c r="K1" s="101"/>
+      <c r="L1" s="101"/>
     </row>
     <row r="2" spans="2:12">
-      <c r="B2" s="88"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
+      <c r="B2" s="103"/>
+      <c r="C2" s="104"/>
+      <c r="D2" s="104"/>
+      <c r="E2" s="104"/>
+      <c r="F2" s="104"/>
+      <c r="G2" s="104"/>
+      <c r="H2" s="104"/>
+      <c r="I2" s="104"/>
+      <c r="J2" s="104"/>
+      <c r="K2" s="104"/>
+      <c r="L2" s="104"/>
     </row>
     <row r="3" spans="2:12" ht="44.25" customHeight="1">
-      <c r="B3" s="87" t="s">
+      <c r="B3" s="102" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="87" t="s">
+      <c r="C3" s="102" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="87" t="s">
+      <c r="D3" s="102" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="87" t="s">
+      <c r="E3" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="87" t="s">
+      <c r="F3" s="102" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="90" t="s">
+      <c r="G3" s="105" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="87" t="s">
+      <c r="H3" s="102" t="s">
         <v>8</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="87" t="s">
+      <c r="J3" s="102" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="87"/>
-      <c r="L3" s="87"/>
+      <c r="K3" s="102"/>
+      <c r="L3" s="102"/>
     </row>
     <row r="4" spans="2:12">
-      <c r="B4" s="87"/>
-      <c r="C4" s="87"/>
-      <c r="D4" s="87"/>
-      <c r="E4" s="87"/>
-      <c r="F4" s="87"/>
-      <c r="G4" s="90"/>
-      <c r="H4" s="87"/>
+      <c r="B4" s="102"/>
+      <c r="C4" s="102"/>
+      <c r="D4" s="102"/>
+      <c r="E4" s="102"/>
+      <c r="F4" s="102"/>
+      <c r="G4" s="105"/>
+      <c r="H4" s="102"/>
       <c r="I4" s="2" t="s">
         <v>10</v>
       </c>
@@ -5849,13 +5849,13 @@
       </c>
     </row>
     <row r="5" spans="2:12" ht="16.5" customHeight="1">
-      <c r="B5" s="100" t="s">
+      <c r="B5" s="95" t="s">
         <v>107</v>
       </c>
       <c r="C5" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="93" t="s">
+      <c r="D5" s="88" t="s">
         <v>39</v>
       </c>
       <c r="E5" s="3" t="s">
@@ -5884,11 +5884,11 @@
       </c>
     </row>
     <row r="6" spans="2:12" ht="16.5" customHeight="1">
-      <c r="B6" s="100"/>
+      <c r="B6" s="95"/>
       <c r="C6" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="93"/>
+      <c r="D6" s="88"/>
       <c r="E6" s="3" t="s">
         <v>41</v>
       </c>
@@ -5915,11 +5915,11 @@
       </c>
     </row>
     <row r="7" spans="2:12" ht="16.5" customHeight="1">
-      <c r="B7" s="100"/>
+      <c r="B7" s="95"/>
       <c r="C7" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="93"/>
+      <c r="D7" s="88"/>
       <c r="E7" s="3" t="s">
         <v>42</v>
       </c>
@@ -5946,11 +5946,11 @@
       </c>
     </row>
     <row r="8" spans="2:12" ht="16.5" customHeight="1">
-      <c r="B8" s="100"/>
+      <c r="B8" s="95"/>
       <c r="C8" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="93"/>
+      <c r="D8" s="88"/>
       <c r="E8" s="3" t="s">
         <v>40</v>
       </c>
@@ -5977,11 +5977,11 @@
       </c>
     </row>
     <row r="9" spans="2:12" ht="16.5" customHeight="1">
-      <c r="B9" s="100"/>
+      <c r="B9" s="95"/>
       <c r="C9" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="93"/>
+      <c r="D9" s="88"/>
       <c r="E9" s="3" t="s">
         <v>42</v>
       </c>
@@ -6008,11 +6008,11 @@
       </c>
     </row>
     <row r="10" spans="2:12" ht="16.5" customHeight="1" thickBot="1">
-      <c r="B10" s="101"/>
+      <c r="B10" s="96"/>
       <c r="C10" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="99"/>
+      <c r="D10" s="94"/>
       <c r="E10" s="27" t="s">
         <v>42</v>
       </c>
@@ -6039,13 +6039,13 @@
       </c>
     </row>
     <row r="11" spans="2:12" ht="16.5" customHeight="1">
-      <c r="B11" s="102" t="s">
+      <c r="B11" s="97" t="s">
         <v>108</v>
       </c>
       <c r="C11" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="D11" s="105" t="s">
+      <c r="D11" s="100" t="s">
         <v>56</v>
       </c>
       <c r="E11" s="32" t="s">
@@ -6074,11 +6074,11 @@
       </c>
     </row>
     <row r="12" spans="2:12" ht="16.5" customHeight="1">
-      <c r="B12" s="103"/>
+      <c r="B12" s="98"/>
       <c r="C12" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="D12" s="97"/>
+      <c r="D12" s="92"/>
       <c r="E12" s="3" t="s">
         <v>40</v>
       </c>
@@ -6105,11 +6105,11 @@
       </c>
     </row>
     <row r="13" spans="2:12" ht="16.5" customHeight="1">
-      <c r="B13" s="103"/>
+      <c r="B13" s="98"/>
       <c r="C13" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="97"/>
+      <c r="D13" s="92"/>
       <c r="E13" s="3" t="s">
         <v>41</v>
       </c>
@@ -6136,11 +6136,11 @@
       </c>
     </row>
     <row r="14" spans="2:12" ht="16.5" customHeight="1">
-      <c r="B14" s="103"/>
+      <c r="B14" s="98"/>
       <c r="C14" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="97"/>
+      <c r="D14" s="92"/>
       <c r="E14" s="3" t="s">
         <v>42</v>
       </c>
@@ -6167,11 +6167,11 @@
       </c>
     </row>
     <row r="15" spans="2:12" ht="16.5" customHeight="1">
-      <c r="B15" s="103"/>
+      <c r="B15" s="98"/>
       <c r="C15" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="97"/>
+      <c r="D15" s="92"/>
       <c r="E15" s="3" t="s">
         <v>40</v>
       </c>
@@ -6198,11 +6198,11 @@
       </c>
     </row>
     <row r="16" spans="2:12" ht="16.5" customHeight="1">
-      <c r="B16" s="104"/>
+      <c r="B16" s="99"/>
       <c r="C16" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="98"/>
+      <c r="D16" s="93"/>
       <c r="E16" s="3" t="s">
         <v>42</v>
       </c>
@@ -6229,13 +6229,13 @@
       </c>
     </row>
     <row r="17" spans="2:12" ht="16.5" customHeight="1">
-      <c r="B17" s="95" t="s">
+      <c r="B17" s="90" t="s">
         <v>116</v>
       </c>
       <c r="C17" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="D17" s="97" t="s">
+      <c r="D17" s="92" t="s">
         <v>100</v>
       </c>
       <c r="E17" s="3" t="s">
@@ -6264,11 +6264,11 @@
       </c>
     </row>
     <row r="18" spans="2:12" ht="16.5" customHeight="1">
-      <c r="B18" s="95"/>
+      <c r="B18" s="90"/>
       <c r="C18" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="D18" s="97"/>
+      <c r="D18" s="92"/>
       <c r="E18" s="3" t="s">
         <v>40</v>
       </c>
@@ -6295,11 +6295,11 @@
       </c>
     </row>
     <row r="19" spans="2:12" ht="16.5" customHeight="1">
-      <c r="B19" s="95"/>
+      <c r="B19" s="90"/>
       <c r="C19" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="97"/>
+      <c r="D19" s="92"/>
       <c r="E19" s="3" t="s">
         <v>40</v>
       </c>
@@ -6326,11 +6326,11 @@
       </c>
     </row>
     <row r="20" spans="2:12" ht="16.5" customHeight="1">
-      <c r="B20" s="95"/>
+      <c r="B20" s="90"/>
       <c r="C20" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D20" s="97"/>
+      <c r="D20" s="92"/>
       <c r="E20" s="3" t="s">
         <v>41</v>
       </c>
@@ -6357,11 +6357,11 @@
       </c>
     </row>
     <row r="21" spans="2:12" ht="16.5" customHeight="1">
-      <c r="B21" s="96"/>
+      <c r="B21" s="91"/>
       <c r="C21" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D21" s="98"/>
+      <c r="D21" s="93"/>
       <c r="E21" s="3" t="s">
         <v>41</v>
       </c>
@@ -6388,13 +6388,13 @@
       </c>
     </row>
     <row r="22" spans="2:12">
-      <c r="B22" s="91" t="s">
+      <c r="B22" s="86" t="s">
         <v>111</v>
       </c>
       <c r="C22" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="D22" s="93" t="s">
+      <c r="D22" s="88" t="s">
         <v>105</v>
       </c>
       <c r="E22" s="3" t="s">
@@ -6423,11 +6423,11 @@
       </c>
     </row>
     <row r="23" spans="2:12" ht="16.5" customHeight="1">
-      <c r="B23" s="91"/>
+      <c r="B23" s="86"/>
       <c r="C23" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="D23" s="93"/>
+      <c r="D23" s="88"/>
       <c r="E23" s="3" t="s">
         <v>40</v>
       </c>
@@ -6454,11 +6454,11 @@
       </c>
     </row>
     <row r="24" spans="2:12">
-      <c r="B24" s="91"/>
+      <c r="B24" s="86"/>
       <c r="C24" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="D24" s="93"/>
+      <c r="D24" s="88"/>
       <c r="E24" s="3" t="s">
         <v>40</v>
       </c>
@@ -6485,11 +6485,11 @@
       </c>
     </row>
     <row r="25" spans="2:12" ht="15" thickBot="1">
-      <c r="B25" s="92"/>
+      <c r="B25" s="87"/>
       <c r="C25" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="D25" s="94"/>
+      <c r="D25" s="89"/>
       <c r="E25" s="38" t="s">
         <v>40</v>
       </c>
@@ -6517,14 +6517,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="D22:D25"/>
-    <mergeCell ref="B17:B21"/>
-    <mergeCell ref="D17:D21"/>
-    <mergeCell ref="D5:D10"/>
-    <mergeCell ref="B5:B10"/>
-    <mergeCell ref="B11:B16"/>
-    <mergeCell ref="D11:D16"/>
     <mergeCell ref="B1:L1"/>
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="J3:L3"/>
@@ -6535,6 +6527,14 @@
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="G3:G4"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="D22:D25"/>
+    <mergeCell ref="B17:B21"/>
+    <mergeCell ref="D17:D21"/>
+    <mergeCell ref="D5:D10"/>
+    <mergeCell ref="B5:B10"/>
+    <mergeCell ref="B11:B16"/>
+    <mergeCell ref="D11:D16"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="J16" r:id="rId1" xr:uid="{9ED0CFC7-005B-4683-8FE2-E7E63AEF0604}"/>
@@ -7279,17 +7279,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="I1:M1"/>
+    <mergeCell ref="I9:N9"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="I26:M26"/>
+    <mergeCell ref="I34:M34"/>
     <mergeCell ref="I42:L42"/>
     <mergeCell ref="I49:L49"/>
     <mergeCell ref="I58:K58"/>
     <mergeCell ref="B23:G31"/>
     <mergeCell ref="A9:F12"/>
     <mergeCell ref="B13:G22"/>
-    <mergeCell ref="I1:M1"/>
-    <mergeCell ref="I9:N9"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="I26:M26"/>
-    <mergeCell ref="I34:M34"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="M28" r:id="rId1" xr:uid="{2AEE64C5-4C39-423F-9B8B-B00C18A04932}"/>
@@ -7332,37 +7332,37 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12">
-      <c r="B2" s="86" t="s">
+      <c r="B2" s="101" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="86"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="101"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="101"/>
+      <c r="H2" s="101"/>
+      <c r="I2" s="101"/>
+      <c r="J2" s="101"/>
+      <c r="K2" s="101"/>
+      <c r="L2" s="101"/>
     </row>
     <row r="3" spans="2:12" ht="15" customHeight="1">
-      <c r="B3" s="109" t="s">
+      <c r="B3" s="115" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="109" t="s">
+      <c r="C3" s="115" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="109" t="s">
+      <c r="D3" s="115" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="109" t="s">
+      <c r="E3" s="115" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="110" t="s">
+      <c r="F3" s="116" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="109" t="s">
+      <c r="G3" s="115" t="s">
         <v>20</v>
       </c>
       <c r="H3" s="5" t="s">
@@ -7371,51 +7371,51 @@
       <c r="I3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="109" t="s">
+      <c r="J3" s="115" t="s">
         <v>25</v>
       </c>
-      <c r="K3" s="109" t="s">
+      <c r="K3" s="115" t="s">
         <v>26</v>
       </c>
-      <c r="L3" s="109" t="s">
+      <c r="L3" s="115" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="4" spans="2:12" ht="15.9" customHeight="1">
-      <c r="B4" s="109"/>
-      <c r="C4" s="109"/>
-      <c r="D4" s="109"/>
-      <c r="E4" s="109"/>
-      <c r="F4" s="111"/>
-      <c r="G4" s="109"/>
-      <c r="H4" s="113" t="s">
+      <c r="B4" s="115"/>
+      <c r="C4" s="115"/>
+      <c r="D4" s="115"/>
+      <c r="E4" s="115"/>
+      <c r="F4" s="117"/>
+      <c r="G4" s="115"/>
+      <c r="H4" s="119" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="114"/>
-      <c r="J4" s="109"/>
-      <c r="K4" s="109"/>
-      <c r="L4" s="109"/>
+      <c r="I4" s="120"/>
+      <c r="J4" s="115"/>
+      <c r="K4" s="115"/>
+      <c r="L4" s="115"/>
     </row>
     <row r="5" spans="2:12">
-      <c r="B5" s="109"/>
-      <c r="C5" s="109"/>
-      <c r="D5" s="109"/>
-      <c r="E5" s="109"/>
-      <c r="F5" s="112"/>
-      <c r="G5" s="109"/>
+      <c r="B5" s="115"/>
+      <c r="C5" s="115"/>
+      <c r="D5" s="115"/>
+      <c r="E5" s="115"/>
+      <c r="F5" s="118"/>
+      <c r="G5" s="115"/>
       <c r="H5" s="5" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="6"/>
-      <c r="J5" s="109"/>
-      <c r="K5" s="109"/>
-      <c r="L5" s="109"/>
+      <c r="J5" s="115"/>
+      <c r="K5" s="115"/>
+      <c r="L5" s="115"/>
     </row>
     <row r="6" spans="2:12">
-      <c r="B6" s="115" t="s">
+      <c r="B6" s="109" t="s">
         <v>77</v>
       </c>
-      <c r="C6" s="118" t="s">
+      <c r="C6" s="112" t="s">
         <v>107</v>
       </c>
       <c r="D6" s="8" t="s">
@@ -7445,8 +7445,8 @@
       <c r="L6" s="7"/>
     </row>
     <row r="7" spans="2:12">
-      <c r="B7" s="116"/>
-      <c r="C7" s="119"/>
+      <c r="B7" s="110"/>
+      <c r="C7" s="113"/>
       <c r="D7" s="8" t="s">
         <v>78</v>
       </c>
@@ -7474,8 +7474,8 @@
       <c r="L7" s="7"/>
     </row>
     <row r="8" spans="2:12">
-      <c r="B8" s="117"/>
-      <c r="C8" s="120"/>
+      <c r="B8" s="111"/>
+      <c r="C8" s="114"/>
       <c r="D8" s="8" t="s">
         <v>78</v>
       </c>
@@ -7503,10 +7503,10 @@
       <c r="L8" s="7"/>
     </row>
     <row r="9" spans="2:12">
-      <c r="B9" s="115" t="s">
+      <c r="B9" s="109" t="s">
         <v>89</v>
       </c>
-      <c r="C9" s="118" t="s">
+      <c r="C9" s="112" t="s">
         <v>108</v>
       </c>
       <c r="D9" s="8" t="s">
@@ -7536,8 +7536,8 @@
       <c r="L9" s="7"/>
     </row>
     <row r="10" spans="2:12">
-      <c r="B10" s="117"/>
-      <c r="C10" s="120"/>
+      <c r="B10" s="111"/>
+      <c r="C10" s="114"/>
       <c r="D10" s="8" t="s">
         <v>78</v>
       </c>
@@ -7565,10 +7565,10 @@
       <c r="L10" s="7"/>
     </row>
     <row r="11" spans="2:12">
-      <c r="B11" s="115" t="s">
+      <c r="B11" s="109" t="s">
         <v>93</v>
       </c>
-      <c r="C11" s="118" t="s">
+      <c r="C11" s="112" t="s">
         <v>109</v>
       </c>
       <c r="D11" s="8" t="s">
@@ -7598,8 +7598,8 @@
       <c r="L11" s="7"/>
     </row>
     <row r="12" spans="2:12">
-      <c r="B12" s="116"/>
-      <c r="C12" s="119"/>
+      <c r="B12" s="110"/>
+      <c r="C12" s="113"/>
       <c r="D12" s="8" t="s">
         <v>78</v>
       </c>
@@ -7627,8 +7627,8 @@
       <c r="L12" s="7"/>
     </row>
     <row r="13" spans="2:12">
-      <c r="B13" s="117"/>
-      <c r="C13" s="120"/>
+      <c r="B13" s="111"/>
+      <c r="C13" s="114"/>
       <c r="D13" s="8" t="s">
         <v>78</v>
       </c>
@@ -7657,12 +7657,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="C6:C8"/>
     <mergeCell ref="B2:L2"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="C3:C5"/>
@@ -7674,6 +7668,12 @@
     <mergeCell ref="J3:J5"/>
     <mergeCell ref="K3:K5"/>
     <mergeCell ref="L3:L5"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="C6:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
TODAS LAS TABLAS ESTAN FUNCIONANDO
</commit_message>
<xml_diff>
--- a/src/main/resources/db/1.xlsx
+++ b/src/main/resources/db/1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dev\GIT\sisfubackend\src\main\resources\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1043787C-99C4-49D1-B249-97CE551A4837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA9BCF08-D40E-4588-92BC-B1AD3DEFD700}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="769" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1553,6 +1553,21 @@
     <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1598,21 +1613,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1622,6 +1622,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1639,24 +1657,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3793,24 +3793,24 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A33:A38"/>
+    <mergeCell ref="B33:B38"/>
+    <mergeCell ref="C33:C38"/>
+    <mergeCell ref="A39:A44"/>
+    <mergeCell ref="B39:B44"/>
+    <mergeCell ref="C39:C44"/>
+    <mergeCell ref="C3:C14"/>
+    <mergeCell ref="A3:A14"/>
+    <mergeCell ref="B3:B14"/>
+    <mergeCell ref="A15:A20"/>
+    <mergeCell ref="B15:B20"/>
+    <mergeCell ref="C15:C20"/>
     <mergeCell ref="A27:A32"/>
     <mergeCell ref="B27:B32"/>
     <mergeCell ref="C27:C32"/>
     <mergeCell ref="A21:A26"/>
     <mergeCell ref="B21:B26"/>
     <mergeCell ref="C21:C26"/>
-    <mergeCell ref="C3:C14"/>
-    <mergeCell ref="A3:A14"/>
-    <mergeCell ref="B3:B14"/>
-    <mergeCell ref="A15:A20"/>
-    <mergeCell ref="B15:B20"/>
-    <mergeCell ref="C15:C20"/>
-    <mergeCell ref="A33:A38"/>
-    <mergeCell ref="B33:B38"/>
-    <mergeCell ref="C33:C38"/>
-    <mergeCell ref="A39:A44"/>
-    <mergeCell ref="B39:B44"/>
-    <mergeCell ref="C39:C44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3822,9 +3822,9 @@
   <dimension ref="A1:W37"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="95" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="A17" sqref="A17:XFD17"/>
+      <selection pane="topRight" activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -5769,72 +5769,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="37.5" customHeight="1">
-      <c r="B1" s="101" t="s">
+      <c r="B1" s="86" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="101"/>
-      <c r="D1" s="101"/>
-      <c r="E1" s="101"/>
-      <c r="F1" s="101"/>
-      <c r="G1" s="101"/>
-      <c r="H1" s="101"/>
-      <c r="I1" s="101"/>
-      <c r="J1" s="101"/>
-      <c r="K1" s="101"/>
-      <c r="L1" s="101"/>
+      <c r="C1" s="86"/>
+      <c r="D1" s="86"/>
+      <c r="E1" s="86"/>
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="86"/>
+      <c r="K1" s="86"/>
+      <c r="L1" s="86"/>
     </row>
     <row r="2" spans="2:12">
-      <c r="B2" s="103"/>
-      <c r="C2" s="104"/>
-      <c r="D2" s="104"/>
-      <c r="E2" s="104"/>
-      <c r="F2" s="104"/>
-      <c r="G2" s="104"/>
-      <c r="H2" s="104"/>
-      <c r="I2" s="104"/>
-      <c r="J2" s="104"/>
-      <c r="K2" s="104"/>
-      <c r="L2" s="104"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="89"/>
+      <c r="K2" s="89"/>
+      <c r="L2" s="89"/>
     </row>
     <row r="3" spans="2:12" ht="44.25" customHeight="1">
-      <c r="B3" s="102" t="s">
+      <c r="B3" s="87" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="102" t="s">
+      <c r="C3" s="87" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="102" t="s">
+      <c r="D3" s="87" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="102" t="s">
+      <c r="E3" s="87" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="102" t="s">
+      <c r="F3" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="105" t="s">
+      <c r="G3" s="90" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="102" t="s">
+      <c r="H3" s="87" t="s">
         <v>8</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="102" t="s">
+      <c r="J3" s="87" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="102"/>
-      <c r="L3" s="102"/>
+      <c r="K3" s="87"/>
+      <c r="L3" s="87"/>
     </row>
     <row r="4" spans="2:12">
-      <c r="B4" s="102"/>
-      <c r="C4" s="102"/>
-      <c r="D4" s="102"/>
-      <c r="E4" s="102"/>
-      <c r="F4" s="102"/>
-      <c r="G4" s="105"/>
-      <c r="H4" s="102"/>
+      <c r="B4" s="87"/>
+      <c r="C4" s="87"/>
+      <c r="D4" s="87"/>
+      <c r="E4" s="87"/>
+      <c r="F4" s="87"/>
+      <c r="G4" s="90"/>
+      <c r="H4" s="87"/>
       <c r="I4" s="2" t="s">
         <v>10</v>
       </c>
@@ -5849,13 +5849,13 @@
       </c>
     </row>
     <row r="5" spans="2:12" ht="16.5" customHeight="1">
-      <c r="B5" s="95" t="s">
+      <c r="B5" s="100" t="s">
         <v>107</v>
       </c>
       <c r="C5" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="88" t="s">
+      <c r="D5" s="93" t="s">
         <v>39</v>
       </c>
       <c r="E5" s="3" t="s">
@@ -5884,11 +5884,11 @@
       </c>
     </row>
     <row r="6" spans="2:12" ht="16.5" customHeight="1">
-      <c r="B6" s="95"/>
+      <c r="B6" s="100"/>
       <c r="C6" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="88"/>
+      <c r="D6" s="93"/>
       <c r="E6" s="3" t="s">
         <v>41</v>
       </c>
@@ -5915,11 +5915,11 @@
       </c>
     </row>
     <row r="7" spans="2:12" ht="16.5" customHeight="1">
-      <c r="B7" s="95"/>
+      <c r="B7" s="100"/>
       <c r="C7" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="88"/>
+      <c r="D7" s="93"/>
       <c r="E7" s="3" t="s">
         <v>42</v>
       </c>
@@ -5946,11 +5946,11 @@
       </c>
     </row>
     <row r="8" spans="2:12" ht="16.5" customHeight="1">
-      <c r="B8" s="95"/>
+      <c r="B8" s="100"/>
       <c r="C8" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="88"/>
+      <c r="D8" s="93"/>
       <c r="E8" s="3" t="s">
         <v>40</v>
       </c>
@@ -5977,11 +5977,11 @@
       </c>
     </row>
     <row r="9" spans="2:12" ht="16.5" customHeight="1">
-      <c r="B9" s="95"/>
+      <c r="B9" s="100"/>
       <c r="C9" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="88"/>
+      <c r="D9" s="93"/>
       <c r="E9" s="3" t="s">
         <v>42</v>
       </c>
@@ -6008,11 +6008,11 @@
       </c>
     </row>
     <row r="10" spans="2:12" ht="16.5" customHeight="1" thickBot="1">
-      <c r="B10" s="96"/>
+      <c r="B10" s="101"/>
       <c r="C10" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="94"/>
+      <c r="D10" s="99"/>
       <c r="E10" s="27" t="s">
         <v>42</v>
       </c>
@@ -6039,13 +6039,13 @@
       </c>
     </row>
     <row r="11" spans="2:12" ht="16.5" customHeight="1">
-      <c r="B11" s="97" t="s">
+      <c r="B11" s="102" t="s">
         <v>108</v>
       </c>
       <c r="C11" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="D11" s="100" t="s">
+      <c r="D11" s="105" t="s">
         <v>56</v>
       </c>
       <c r="E11" s="32" t="s">
@@ -6074,11 +6074,11 @@
       </c>
     </row>
     <row r="12" spans="2:12" ht="16.5" customHeight="1">
-      <c r="B12" s="98"/>
+      <c r="B12" s="103"/>
       <c r="C12" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="D12" s="92"/>
+      <c r="D12" s="97"/>
       <c r="E12" s="3" t="s">
         <v>40</v>
       </c>
@@ -6105,11 +6105,11 @@
       </c>
     </row>
     <row r="13" spans="2:12" ht="16.5" customHeight="1">
-      <c r="B13" s="98"/>
+      <c r="B13" s="103"/>
       <c r="C13" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="92"/>
+      <c r="D13" s="97"/>
       <c r="E13" s="3" t="s">
         <v>41</v>
       </c>
@@ -6136,11 +6136,11 @@
       </c>
     </row>
     <row r="14" spans="2:12" ht="16.5" customHeight="1">
-      <c r="B14" s="98"/>
+      <c r="B14" s="103"/>
       <c r="C14" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="92"/>
+      <c r="D14" s="97"/>
       <c r="E14" s="3" t="s">
         <v>42</v>
       </c>
@@ -6167,11 +6167,11 @@
       </c>
     </row>
     <row r="15" spans="2:12" ht="16.5" customHeight="1">
-      <c r="B15" s="98"/>
+      <c r="B15" s="103"/>
       <c r="C15" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="92"/>
+      <c r="D15" s="97"/>
       <c r="E15" s="3" t="s">
         <v>40</v>
       </c>
@@ -6198,11 +6198,11 @@
       </c>
     </row>
     <row r="16" spans="2:12" ht="16.5" customHeight="1">
-      <c r="B16" s="99"/>
+      <c r="B16" s="104"/>
       <c r="C16" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="93"/>
+      <c r="D16" s="98"/>
       <c r="E16" s="3" t="s">
         <v>42</v>
       </c>
@@ -6229,13 +6229,13 @@
       </c>
     </row>
     <row r="17" spans="2:12" ht="16.5" customHeight="1">
-      <c r="B17" s="90" t="s">
+      <c r="B17" s="95" t="s">
         <v>116</v>
       </c>
       <c r="C17" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="D17" s="92" t="s">
+      <c r="D17" s="97" t="s">
         <v>100</v>
       </c>
       <c r="E17" s="3" t="s">
@@ -6264,11 +6264,11 @@
       </c>
     </row>
     <row r="18" spans="2:12" ht="16.5" customHeight="1">
-      <c r="B18" s="90"/>
+      <c r="B18" s="95"/>
       <c r="C18" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="D18" s="92"/>
+      <c r="D18" s="97"/>
       <c r="E18" s="3" t="s">
         <v>40</v>
       </c>
@@ -6295,11 +6295,11 @@
       </c>
     </row>
     <row r="19" spans="2:12" ht="16.5" customHeight="1">
-      <c r="B19" s="90"/>
+      <c r="B19" s="95"/>
       <c r="C19" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="92"/>
+      <c r="D19" s="97"/>
       <c r="E19" s="3" t="s">
         <v>40</v>
       </c>
@@ -6326,11 +6326,11 @@
       </c>
     </row>
     <row r="20" spans="2:12" ht="16.5" customHeight="1">
-      <c r="B20" s="90"/>
+      <c r="B20" s="95"/>
       <c r="C20" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D20" s="92"/>
+      <c r="D20" s="97"/>
       <c r="E20" s="3" t="s">
         <v>41</v>
       </c>
@@ -6357,11 +6357,11 @@
       </c>
     </row>
     <row r="21" spans="2:12" ht="16.5" customHeight="1">
-      <c r="B21" s="91"/>
+      <c r="B21" s="96"/>
       <c r="C21" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D21" s="93"/>
+      <c r="D21" s="98"/>
       <c r="E21" s="3" t="s">
         <v>41</v>
       </c>
@@ -6388,13 +6388,13 @@
       </c>
     </row>
     <row r="22" spans="2:12">
-      <c r="B22" s="86" t="s">
+      <c r="B22" s="91" t="s">
         <v>111</v>
       </c>
       <c r="C22" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="D22" s="88" t="s">
+      <c r="D22" s="93" t="s">
         <v>105</v>
       </c>
       <c r="E22" s="3" t="s">
@@ -6423,11 +6423,11 @@
       </c>
     </row>
     <row r="23" spans="2:12" ht="16.5" customHeight="1">
-      <c r="B23" s="86"/>
+      <c r="B23" s="91"/>
       <c r="C23" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="D23" s="88"/>
+      <c r="D23" s="93"/>
       <c r="E23" s="3" t="s">
         <v>40</v>
       </c>
@@ -6454,11 +6454,11 @@
       </c>
     </row>
     <row r="24" spans="2:12">
-      <c r="B24" s="86"/>
+      <c r="B24" s="91"/>
       <c r="C24" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="D24" s="88"/>
+      <c r="D24" s="93"/>
       <c r="E24" s="3" t="s">
         <v>40</v>
       </c>
@@ -6485,11 +6485,11 @@
       </c>
     </row>
     <row r="25" spans="2:12" ht="15" thickBot="1">
-      <c r="B25" s="87"/>
+      <c r="B25" s="92"/>
       <c r="C25" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="D25" s="89"/>
+      <c r="D25" s="94"/>
       <c r="E25" s="38" t="s">
         <v>40</v>
       </c>
@@ -6517,6 +6517,14 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="D22:D25"/>
+    <mergeCell ref="B17:B21"/>
+    <mergeCell ref="D17:D21"/>
+    <mergeCell ref="D5:D10"/>
+    <mergeCell ref="B5:B10"/>
+    <mergeCell ref="B11:B16"/>
+    <mergeCell ref="D11:D16"/>
     <mergeCell ref="B1:L1"/>
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="J3:L3"/>
@@ -6527,14 +6535,6 @@
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="G3:G4"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="D22:D25"/>
-    <mergeCell ref="B17:B21"/>
-    <mergeCell ref="D17:D21"/>
-    <mergeCell ref="D5:D10"/>
-    <mergeCell ref="B5:B10"/>
-    <mergeCell ref="B11:B16"/>
-    <mergeCell ref="D11:D16"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="J16" r:id="rId1" xr:uid="{9ED0CFC7-005B-4683-8FE2-E7E63AEF0604}"/>
@@ -7279,17 +7279,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="I1:M1"/>
-    <mergeCell ref="I9:N9"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="I26:M26"/>
-    <mergeCell ref="I34:M34"/>
     <mergeCell ref="I42:L42"/>
     <mergeCell ref="I49:L49"/>
     <mergeCell ref="I58:K58"/>
     <mergeCell ref="B23:G31"/>
     <mergeCell ref="A9:F12"/>
     <mergeCell ref="B13:G22"/>
+    <mergeCell ref="I1:M1"/>
+    <mergeCell ref="I9:N9"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="I26:M26"/>
+    <mergeCell ref="I34:M34"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="M28" r:id="rId1" xr:uid="{2AEE64C5-4C39-423F-9B8B-B00C18A04932}"/>
@@ -7332,37 +7332,37 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12">
-      <c r="B2" s="101" t="s">
+      <c r="B2" s="86" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="101"/>
-      <c r="D2" s="101"/>
-      <c r="E2" s="101"/>
-      <c r="F2" s="101"/>
-      <c r="G2" s="101"/>
-      <c r="H2" s="101"/>
-      <c r="I2" s="101"/>
-      <c r="J2" s="101"/>
-      <c r="K2" s="101"/>
-      <c r="L2" s="101"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="86"/>
     </row>
     <row r="3" spans="2:12" ht="15" customHeight="1">
-      <c r="B3" s="115" t="s">
+      <c r="B3" s="109" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="115" t="s">
+      <c r="C3" s="109" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="115" t="s">
+      <c r="D3" s="109" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="115" t="s">
+      <c r="E3" s="109" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="116" t="s">
+      <c r="F3" s="110" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="115" t="s">
+      <c r="G3" s="109" t="s">
         <v>20</v>
       </c>
       <c r="H3" s="5" t="s">
@@ -7371,51 +7371,51 @@
       <c r="I3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="115" t="s">
+      <c r="J3" s="109" t="s">
         <v>25</v>
       </c>
-      <c r="K3" s="115" t="s">
+      <c r="K3" s="109" t="s">
         <v>26</v>
       </c>
-      <c r="L3" s="115" t="s">
+      <c r="L3" s="109" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="4" spans="2:12" ht="15.9" customHeight="1">
-      <c r="B4" s="115"/>
-      <c r="C4" s="115"/>
-      <c r="D4" s="115"/>
-      <c r="E4" s="115"/>
-      <c r="F4" s="117"/>
-      <c r="G4" s="115"/>
-      <c r="H4" s="119" t="s">
+      <c r="B4" s="109"/>
+      <c r="C4" s="109"/>
+      <c r="D4" s="109"/>
+      <c r="E4" s="109"/>
+      <c r="F4" s="111"/>
+      <c r="G4" s="109"/>
+      <c r="H4" s="113" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="120"/>
-      <c r="J4" s="115"/>
-      <c r="K4" s="115"/>
-      <c r="L4" s="115"/>
+      <c r="I4" s="114"/>
+      <c r="J4" s="109"/>
+      <c r="K4" s="109"/>
+      <c r="L4" s="109"/>
     </row>
     <row r="5" spans="2:12">
-      <c r="B5" s="115"/>
-      <c r="C5" s="115"/>
-      <c r="D5" s="115"/>
-      <c r="E5" s="115"/>
-      <c r="F5" s="118"/>
-      <c r="G5" s="115"/>
+      <c r="B5" s="109"/>
+      <c r="C5" s="109"/>
+      <c r="D5" s="109"/>
+      <c r="E5" s="109"/>
+      <c r="F5" s="112"/>
+      <c r="G5" s="109"/>
       <c r="H5" s="5" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="6"/>
-      <c r="J5" s="115"/>
-      <c r="K5" s="115"/>
-      <c r="L5" s="115"/>
+      <c r="J5" s="109"/>
+      <c r="K5" s="109"/>
+      <c r="L5" s="109"/>
     </row>
     <row r="6" spans="2:12">
-      <c r="B6" s="109" t="s">
+      <c r="B6" s="115" t="s">
         <v>77</v>
       </c>
-      <c r="C6" s="112" t="s">
+      <c r="C6" s="118" t="s">
         <v>107</v>
       </c>
       <c r="D6" s="8" t="s">
@@ -7445,8 +7445,8 @@
       <c r="L6" s="7"/>
     </row>
     <row r="7" spans="2:12">
-      <c r="B7" s="110"/>
-      <c r="C7" s="113"/>
+      <c r="B7" s="116"/>
+      <c r="C7" s="119"/>
       <c r="D7" s="8" t="s">
         <v>78</v>
       </c>
@@ -7474,8 +7474,8 @@
       <c r="L7" s="7"/>
     </row>
     <row r="8" spans="2:12">
-      <c r="B8" s="111"/>
-      <c r="C8" s="114"/>
+      <c r="B8" s="117"/>
+      <c r="C8" s="120"/>
       <c r="D8" s="8" t="s">
         <v>78</v>
       </c>
@@ -7503,10 +7503,10 @@
       <c r="L8" s="7"/>
     </row>
     <row r="9" spans="2:12">
-      <c r="B9" s="109" t="s">
+      <c r="B9" s="115" t="s">
         <v>89</v>
       </c>
-      <c r="C9" s="112" t="s">
+      <c r="C9" s="118" t="s">
         <v>108</v>
       </c>
       <c r="D9" s="8" t="s">
@@ -7536,8 +7536,8 @@
       <c r="L9" s="7"/>
     </row>
     <row r="10" spans="2:12">
-      <c r="B10" s="111"/>
-      <c r="C10" s="114"/>
+      <c r="B10" s="117"/>
+      <c r="C10" s="120"/>
       <c r="D10" s="8" t="s">
         <v>78</v>
       </c>
@@ -7565,10 +7565,10 @@
       <c r="L10" s="7"/>
     </row>
     <row r="11" spans="2:12">
-      <c r="B11" s="109" t="s">
+      <c r="B11" s="115" t="s">
         <v>93</v>
       </c>
-      <c r="C11" s="112" t="s">
+      <c r="C11" s="118" t="s">
         <v>109</v>
       </c>
       <c r="D11" s="8" t="s">
@@ -7598,8 +7598,8 @@
       <c r="L11" s="7"/>
     </row>
     <row r="12" spans="2:12">
-      <c r="B12" s="110"/>
-      <c r="C12" s="113"/>
+      <c r="B12" s="116"/>
+      <c r="C12" s="119"/>
       <c r="D12" s="8" t="s">
         <v>78</v>
       </c>
@@ -7627,8 +7627,8 @@
       <c r="L12" s="7"/>
     </row>
     <row r="13" spans="2:12">
-      <c r="B13" s="111"/>
-      <c r="C13" s="114"/>
+      <c r="B13" s="117"/>
+      <c r="C13" s="120"/>
       <c r="D13" s="8" t="s">
         <v>78</v>
       </c>
@@ -7657,6 +7657,12 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="C6:C8"/>
     <mergeCell ref="B2:L2"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="C3:C5"/>
@@ -7668,12 +7674,6 @@
     <mergeCell ref="J3:J5"/>
     <mergeCell ref="K3:K5"/>
     <mergeCell ref="L3:L5"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="C6:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>